<commit_message>
updating condit_highlighting, adding files
</commit_message>
<xml_diff>
--- a/conditional_highlighting.xlsx
+++ b/conditional_highlighting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>books</t>
   </si>
@@ -112,13 +112,64 @@
     <t>j.d. salinger</t>
   </si>
   <si>
+    <t>3.14</t>
+  </si>
+  <si>
+    <t>743273567</t>
+  </si>
+  <si>
+    <t>439136350</t>
+  </si>
+  <si>
+    <t>60837020</t>
+  </si>
+  <si>
+    <t>808514571</t>
+  </si>
+  <si>
     <t>014242417X</t>
   </si>
   <si>
+    <t>142402516</t>
+  </si>
+  <si>
+    <t>525487085</t>
+  </si>
+  <si>
+    <t>385486804</t>
+  </si>
+  <si>
+    <t>1285159454</t>
+  </si>
+  <si>
     <t>hhhhhhhhh</t>
   </si>
   <si>
     <t>kjh;lkj;kl</t>
+  </si>
+  <si>
+    <t>980852233</t>
+  </si>
+  <si>
+    <t>343455345</t>
+  </si>
+  <si>
+    <t>654654</t>
+  </si>
+  <si>
+    <t>65465465</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -506,8 +557,8 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>743273567</v>
+      <c r="D2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -520,11 +571,11 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>439136350</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -537,11 +588,11 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>60837020</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -554,11 +605,11 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
-        <v>808514571</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -572,10 +623,10 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -588,11 +639,11 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7">
-        <v>142402516</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -605,11 +656,11 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8">
-        <v>525487085</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -622,11 +673,11 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9">
-        <v>385486804</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -639,11 +690,11 @@
       <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D10">
-        <v>1285159454</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -657,10 +708,10 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -674,10 +725,10 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -690,11 +741,11 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="D13">
-        <v>980852233</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -707,11 +758,11 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D14">
-        <v>343455345</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -724,11 +775,11 @@
       <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15">
-        <v>654654</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -741,11 +792,11 @@
       <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="D16">
-        <v>65465465</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -755,14 +806,14 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
-        <v>3.14</v>
-      </c>
-      <c r="D17">
-        <v>142402516</v>
-      </c>
-      <c r="E17">
-        <v>6</v>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>